<commit_message>
Bug Fixes for Issues 26 - 32
Bug Fixes for Issues 26 - 32
</commit_message>
<xml_diff>
--- a/COBiePlugins/lib/COBieDesignTemplate.xlsx
+++ b/COBiePlugins/lib/COBieDesignTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="495" windowWidth="18255" windowHeight="11955" tabRatio="835"/>
+    <workbookView xWindow="150" yWindow="495" windowWidth="18255" windowHeight="11955" tabRatio="835" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="1" r:id="rId1"/>
@@ -16655,6 +16655,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\Thh:mm:ss"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -17263,7 +17266,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -17291,6 +17294,11 @@
     <xf numFmtId="0" fontId="19" fillId="38" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90" shrinkToFit="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90" shrinkToFit="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -17645,7 +17653,7 @@
   </sheetPr>
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17658,64 +17666,64 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="22">
         <v>2</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="22">
         <v>4</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="23"/>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:3" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -18071,14 +18079,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="7" width="9.42578125" style="7" customWidth="1"/>
     <col min="8" max="10" width="9.42578125" style="8" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" style="6" customWidth="1"/>
@@ -18091,7 +18099,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -18126,7 +18134,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -18185,14 +18193,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="10" width="9.42578125" style="7" customWidth="1"/>
     <col min="11" max="13" width="9.42578125" style="8" customWidth="1"/>
     <col min="14" max="14" width="9.42578125" style="6" customWidth="1"/>
@@ -18205,7 +18213,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -18249,7 +18257,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -18314,14 +18322,15 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="15" customWidth="1"/>
-    <col min="3" max="12" width="9.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="21" customWidth="1"/>
+    <col min="4" max="12" width="9.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="130.35" customHeight="1" x14ac:dyDescent="0.25">
@@ -18331,7 +18340,7 @@
       <c r="B1" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="16" t="s">
@@ -18369,7 +18378,7 @@
       <c r="B2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="21" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -18431,12 +18440,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="9.42578125" style="5" customWidth="1"/>
+    <col min="1" max="2" width="9.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="21" customWidth="1"/>
+    <col min="4" max="8" width="9.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="130.35" customHeight="1" x14ac:dyDescent="0.25">
@@ -18446,7 +18457,7 @@
       <c r="B1" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="16" t="s">
@@ -18472,7 +18483,7 @@
       <c r="B2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="21" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -18519,12 +18530,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="19" width="9.42578125" style="5" customWidth="1"/>
+    <col min="1" max="2" width="9.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="21" customWidth="1"/>
+    <col min="4" max="19" width="9.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="130.35" customHeight="1" x14ac:dyDescent="0.25">
@@ -18534,7 +18547,7 @@
       <c r="B1" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="16" t="s">
@@ -18593,7 +18606,7 @@
       <c r="B2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="21" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -18688,12 +18701,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16" width="9.42578125" style="5" customWidth="1"/>
+    <col min="1" max="2" width="9.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="21" customWidth="1"/>
+    <col min="4" max="16" width="9.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="130.35" customHeight="1" x14ac:dyDescent="0.25">
@@ -18703,7 +18718,7 @@
       <c r="B1" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="16" t="s">
@@ -18753,7 +18768,7 @@
       <c r="B2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="21" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -18833,14 +18848,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="8" width="9.42578125" style="7" customWidth="1"/>
     <col min="9" max="10" width="9.42578125" style="4" customWidth="1"/>
     <col min="11" max="13" width="9.42578125" style="8" customWidth="1"/>
@@ -18854,7 +18869,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -18901,7 +18916,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -18974,18 +18989,18 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="6" width="9.42578125" style="7" customWidth="1"/>
     <col min="7" max="8" width="9.42578125" style="4" customWidth="1"/>
     <col min="9" max="11" width="9.42578125" style="8" customWidth="1"/>
@@ -18999,7 +19014,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -19040,7 +19055,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -19105,12 +19120,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="9.42578125" style="15" customWidth="1"/>
+    <col min="1" max="2" width="9.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="21" customWidth="1"/>
+    <col min="4" max="15" width="9.42578125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="130.35" customHeight="1" x14ac:dyDescent="0.25">
@@ -19120,7 +19137,7 @@
       <c r="B1" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="17" t="s">
@@ -19167,7 +19184,7 @@
       <c r="B2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="21" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="15" t="s">
@@ -19238,12 +19255,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="17" width="9.42578125" style="15" customWidth="1"/>
+    <col min="1" max="2" width="9.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="21" customWidth="1"/>
+    <col min="4" max="17" width="9.42578125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="130.35" customHeight="1" x14ac:dyDescent="0.25">
@@ -19253,7 +19272,7 @@
       <c r="B1" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="17" t="s">
@@ -19306,7 +19325,7 @@
       <c r="B2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="21" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="15" t="s">
@@ -19392,14 +19411,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" style="7" customWidth="1"/>
     <col min="5" max="6" width="9.42578125" style="4" customWidth="1"/>
     <col min="7" max="9" width="9.42578125" style="8" customWidth="1"/>
@@ -19413,7 +19432,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -19472,7 +19491,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -19538,6 +19557,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -42222,14 +42242,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" style="7" customWidth="1"/>
     <col min="5" max="6" width="9.42578125" style="4" customWidth="1"/>
     <col min="7" max="10" width="9.42578125" style="7" customWidth="1"/>
@@ -42245,7 +42265,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -42313,7 +42333,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -42420,14 +42440,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" style="7" customWidth="1"/>
     <col min="5" max="7" width="9.42578125" style="8" customWidth="1"/>
     <col min="8" max="10" width="9.42578125" style="6" customWidth="1"/>
@@ -42440,7 +42460,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -42472,7 +42492,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -42525,14 +42545,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="5" width="9.42578125" style="7" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" style="4" customWidth="1"/>
     <col min="7" max="9" width="9.42578125" style="8" customWidth="1"/>
@@ -42547,7 +42567,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -42588,7 +42608,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -42653,14 +42673,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="5" width="9.42578125" style="7" customWidth="1"/>
     <col min="6" max="8" width="9.42578125" style="8" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" style="6" customWidth="1"/>
@@ -42673,7 +42693,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -42702,7 +42722,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -42755,14 +42775,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" style="7" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" style="7" customWidth="1"/>
@@ -42779,7 +42799,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -42886,7 +42906,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -43020,18 +43040,20 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="5" width="9.42578125" style="7" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" style="4" customWidth="1"/>
     <col min="7" max="9" width="9.42578125" style="8" customWidth="1"/>
-    <col min="10" max="15" width="9.42578125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="15" customWidth="1"/>
+    <col min="11" max="12" width="9.42578125" style="21" customWidth="1"/>
+    <col min="13" max="15" width="9.42578125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="130.35" customHeight="1" x14ac:dyDescent="0.25">
@@ -43041,7 +43063,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -43065,10 +43087,10 @@
       <c r="J1" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="19" t="s">
         <v>153</v>
       </c>
       <c r="M1" s="14" t="s">
@@ -43088,7 +43110,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -43112,10 +43134,10 @@
       <c r="J2" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="21" t="s">
         <v>153</v>
       </c>
       <c r="M2" s="15" t="s">
@@ -43159,14 +43181,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="20" customWidth="1"/>
     <col min="4" max="5" width="9.42578125" style="7" customWidth="1"/>
     <col min="6" max="8" width="9.42578125" style="8" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" style="6" customWidth="1"/>
@@ -43179,7 +43201,7 @@
       <c r="B1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="14" t="s">
@@ -43208,7 +43230,7 @@
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">

</xml_diff>